<commit_message>
modif dossier de projet
ajout du journal de travail au dossier de projet
</commit_message>
<xml_diff>
--- a/Journal de travail - YFA.xlsx
+++ b/Journal de travail - YFA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yann7\Documents\GitHub\Bataille-Navale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B9FBE0-BEFD-4277-B22B-4F9077E11B76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881B1BED-C828-4562-BA76-14FDB00FD39D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6171875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>